<commit_message>
Interrupts on pins PC1, PA8, PA9
Pins configured as external interrupts. Pull-up resistors added to pins PA8 and PA9.
Changes added into excel sheet.
</commit_message>
<xml_diff>
--- a/Pinbeschreibung.xlsx
+++ b/Pinbeschreibung.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timynator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clara\Documents\Hardwarenahe Softwareentwicklung\Miniprojekt\Gitkraken_repo\Aquarium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{965D3AFE-EE29-45D3-8D97-0F79FE6C58CA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABA3580-F996-4848-8E98-E1A91A947F3E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{4F45077C-4A2D-4FF2-B245-A517773CDB27}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
   <si>
     <t>Arduino Pin</t>
   </si>
@@ -145,14 +145,34 @@
   </si>
   <si>
     <t>Button in</t>
+  </si>
+  <si>
+    <t>GPIO Pull-up/pull-down</t>
+  </si>
+  <si>
+    <t>pull-up</t>
+  </si>
+  <si>
+    <t>NVIC interrupt table</t>
+  </si>
+  <si>
+    <t>enabled</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -180,8 +200,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -496,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E63E90E0-A7F2-46B3-8DA3-AAB638C7D117}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,23 +529,31 @@
     <col min="2" max="2" width="20.88671875" customWidth="1"/>
     <col min="3" max="3" width="21.109375" customWidth="1"/>
     <col min="4" max="4" width="22.5546875" customWidth="1"/>
+    <col min="5" max="5" width="23.21875" customWidth="1"/>
+    <col min="6" max="6" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -538,7 +567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -552,7 +581,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -566,7 +595,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -580,7 +609,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -594,7 +623,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -608,7 +637,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -622,7 +651,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -636,7 +665,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -649,8 +678,14 @@
       <c r="D10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -663,8 +698,14 @@
       <c r="D11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -677,8 +718,12 @@
       <c r="D12" t="s">
         <v>37</v>
       </c>
+      <c r="F12" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Switch-case for interrupt flag improved
However, still not finished
</commit_message>
<xml_diff>
--- a/Pinbeschreibung.xlsx
+++ b/Pinbeschreibung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clara\Documents\Hardwarenahe Softwareentwicklung\Miniprojekt\Git_repo\Aquarium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A98EC8-99B4-4F15-A36B-965D42967144}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460DC499-7777-4DD3-A6BF-FE2D1E7F9429}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{4F45077C-4A2D-4FF2-B245-A517773CDB27}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
   <si>
     <t>Arduino Pin</t>
   </si>
@@ -141,9 +141,6 @@
     <t>Extern Interrupt</t>
   </si>
   <si>
-    <t>Rotary encoder</t>
-  </si>
-  <si>
     <t>Button in</t>
   </si>
   <si>
@@ -160,6 +157,42 @@
   </si>
   <si>
     <t>pull-down</t>
+  </si>
+  <si>
+    <t>Port: GPIOx</t>
+  </si>
+  <si>
+    <t>Pin: GPIO_PIN_x</t>
+  </si>
+  <si>
+    <t>GPIO_PIN_1</t>
+  </si>
+  <si>
+    <t>GPIOC</t>
+  </si>
+  <si>
+    <t>Rotary encoder channel A</t>
+  </si>
+  <si>
+    <t>GPIOA</t>
+  </si>
+  <si>
+    <t>GPIO_PIN_9</t>
+  </si>
+  <si>
+    <t>GPIO_PIN_8</t>
+  </si>
+  <si>
+    <t>Rotary encoder channel B</t>
+  </si>
+  <si>
+    <t>GPIOB</t>
+  </si>
+  <si>
+    <t>GPIO_PIN_5</t>
+  </si>
+  <si>
+    <t>GPIO_PIN_6</t>
   </si>
 </sst>
 </file>
@@ -520,23 +553,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E63E90E0-A7F2-46B3-8DA3-AAB638C7D117}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" customWidth="1"/>
-    <col min="5" max="5" width="23.21875" customWidth="1"/>
-    <col min="6" max="6" width="23.77734375" customWidth="1"/>
+    <col min="2" max="4" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="23.109375" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" customWidth="1"/>
+    <col min="7" max="7" width="23.21875" customWidth="1"/>
+    <col min="8" max="8" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,103 +577,109 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -648,13 +687,19 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -662,13 +707,19 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -676,19 +727,25 @@
         <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
         <v>37</v>
       </c>
-      <c r="E10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -696,19 +753,25 @@
         <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" t="s">
         <v>37</v>
       </c>
-      <c r="E11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -716,16 +779,22 @@
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
         <v>37</v>
       </c>
-      <c r="E12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>43</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>